<commit_message>
FEAT(OpenWeatherMap) : 기상청 체크 완료 OWM API 도시정보 파일 추가
</commit_message>
<xml_diff>
--- a/Doc/기상API체크리스트.xlsx
+++ b/Doc/기상API체크리스트.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23628"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23801"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\quber\Desktop\Study\weather-vue\Doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BC09D53F-8A14-4C26-A23A-6EF4234B730E}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B01A517B-832D-4FC2-B1B9-6A0E8C0C65DC}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3468" yWindow="456" windowWidth="20496" windowHeight="10656" xr2:uid="{1069D393-E97E-4CFA-8AFF-569F9A233692}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{1069D393-E97E-4CFA-8AFF-569F9A233692}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="72">
   <si>
     <t>기상 정보 API 체크리스트</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -880,6 +880,309 @@
     <t>지역 입력시 한글 인코딩 필요
 api요청시간에서 가장 가까운 최신 데이터 return
 등급 값 : 1 = 좋음 2 = 보통 3 = 나쁨 4 = 매우나쁨</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>API Key</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>422JryGS9%2B676hcl7wOZ4jh5de2s99vCJr2NcRWV4YXkv9nQP8C0BFGDPVlBt55Fyy5VMJh%2ByRYBMkV%2BcciYZg%3D%3D</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>http://apis.data.go.kr/B552584/ArpltnInforInqireSvc/getMinuDustWeekFrcstDspth?searchDate=</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>${date}</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="맑은 고딕"/>
+        <family val="2"/>
+        <charset val="129"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>&amp;returnType=json&amp;serviceKey=</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>${apiKey}</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="맑은 고딕"/>
+        <family val="2"/>
+        <charset val="129"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>&amp;numOfRows=50&amp;pageNo=1</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>frcstOneCn</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>날짜 형식 : YYYY-MM-DD</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>http://apis.data.go.kr/1360000/VilageFcstInfoService/getVilageFcst?serviceKey=</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>${1}</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="맑은 고딕"/>
+        <family val="2"/>
+        <charset val="129"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>&amp;numOfRows=10&amp;pageNo=1&amp;dataType=json&amp;base_date=</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>${2}</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="맑은 고딕"/>
+        <family val="2"/>
+        <charset val="129"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>&amp;base_time=</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>${3}</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="맑은 고딕"/>
+        <family val="2"/>
+        <charset val="129"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>&amp;nx=</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>${4}</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="맑은 고딕"/>
+        <family val="2"/>
+        <charset val="129"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>&amp;ny=</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>${4}</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>주간 강수확률</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>http://apis.data.go.kr/1360000/MidFcstInfoService/getMidLandFcst?serviceKey=</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>${apiKey}</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="맑은 고딕"/>
+        <family val="2"/>
+        <charset val="129"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>&amp;numOfRows=10&amp;pageNo=1&amp;dataType=json&amp;regId=</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>${district}</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="맑은 고딕"/>
+        <family val="2"/>
+        <charset val="129"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>&amp;tmFc=</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>${date}</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>날짜 형식 : yyyymmddhhmm
+주간 기상 정보가 3일 후 부터 가능함
+지역은 한글 가이드문서 참조</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>http://apis.data.go.kr/1360000/MidFcstInfoService/getMidTa?serviceKey=</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>${apiKey}</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="맑은 고딕"/>
+        <family val="2"/>
+        <charset val="129"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>&amp;numOfRows=10&amp;pageNo=1&amp;dataType=json&amp;regId=</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>${district}</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="맑은 고딕"/>
+        <family val="2"/>
+        <charset val="129"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>&amp;tmFc=</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>${date}</t>
+    </r>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -887,7 +1190,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -936,8 +1239,16 @@
       <charset val="129"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <name val="맑은 고딕"/>
+      <family val="3"/>
+      <charset val="129"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -956,8 +1267,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="19">
+  <borders count="20">
     <border>
       <left/>
       <right/>
@@ -1170,8 +1487,21 @@
         <color theme="2" tint="-9.9978637043366805E-2"/>
       </right>
       <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFA7A7A7"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFA7A7A7"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFA7A7A7"/>
+      </top>
       <bottom style="thin">
-        <color theme="2" tint="-9.9978637043366805E-2"/>
+        <color rgb="FFA7A7A7"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1181,7 +1511,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="72">
+  <cellXfs count="91">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -1227,6 +1557,132 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1243,15 +1699,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1260,143 +1707,83 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="19" xfId="0" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1717,10 +2104,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{41B938B0-E336-423D-A499-D7B70BBAC71A}">
-  <dimension ref="A1:V36"/>
+  <dimension ref="A1:W38"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="D28" sqref="D28:P28"/>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="65" zoomScaleNormal="65" workbookViewId="0">
+      <selection activeCell="I29" sqref="I29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.4"/>
@@ -1741,33 +2128,33 @@
     <col min="23" max="16384" width="8.796875" style="6"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:22" s="4" customFormat="1" ht="55.5" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A1" s="18" t="s">
+    <row r="1" spans="1:23" s="4" customFormat="1" ht="55.5" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A1" s="60" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="19"/>
-      <c r="C1" s="19"/>
-      <c r="D1" s="19"/>
-      <c r="E1" s="19"/>
-      <c r="F1" s="19"/>
-      <c r="G1" s="19"/>
-      <c r="H1" s="19"/>
-      <c r="I1" s="19"/>
-      <c r="J1" s="19"/>
-      <c r="K1" s="19"/>
-      <c r="L1" s="19"/>
-      <c r="M1" s="19"/>
-      <c r="N1" s="19"/>
-      <c r="O1" s="19"/>
-      <c r="P1" s="19"/>
-      <c r="Q1" s="20"/>
+      <c r="B1" s="61"/>
+      <c r="C1" s="61"/>
+      <c r="D1" s="61"/>
+      <c r="E1" s="61"/>
+      <c r="F1" s="61"/>
+      <c r="G1" s="61"/>
+      <c r="H1" s="61"/>
+      <c r="I1" s="61"/>
+      <c r="J1" s="61"/>
+      <c r="K1" s="61"/>
+      <c r="L1" s="61"/>
+      <c r="M1" s="61"/>
+      <c r="N1" s="61"/>
+      <c r="O1" s="61"/>
+      <c r="P1" s="61"/>
+      <c r="Q1" s="62"/>
       <c r="R1" s="9"/>
-      <c r="S1" s="48"/>
-      <c r="T1" s="49"/>
-      <c r="U1" s="49"/>
-      <c r="V1" s="50"/>
-    </row>
-    <row r="2" spans="1:22" ht="28.2" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="S1" s="24"/>
+      <c r="T1" s="25"/>
+      <c r="U1" s="25"/>
+      <c r="V1" s="26"/>
+    </row>
+    <row r="2" spans="1:23" ht="28.2" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
@@ -1777,174 +2164,171 @@
       <c r="C2" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="15" t="s">
+      <c r="D2" s="57" t="s">
         <v>4</v>
       </c>
-      <c r="E2" s="16"/>
-      <c r="F2" s="16"/>
-      <c r="G2" s="16"/>
-      <c r="H2" s="16"/>
-      <c r="I2" s="16"/>
-      <c r="J2" s="16"/>
-      <c r="K2" s="16"/>
-      <c r="L2" s="16"/>
-      <c r="M2" s="16"/>
-      <c r="N2" s="16"/>
-      <c r="O2" s="16"/>
-      <c r="P2" s="17"/>
+      <c r="E2" s="58"/>
+      <c r="F2" s="58"/>
+      <c r="G2" s="58"/>
+      <c r="H2" s="58"/>
+      <c r="I2" s="58"/>
+      <c r="J2" s="58"/>
+      <c r="K2" s="58"/>
+      <c r="L2" s="58"/>
+      <c r="M2" s="58"/>
+      <c r="N2" s="58"/>
+      <c r="O2" s="58"/>
+      <c r="P2" s="59"/>
       <c r="Q2" s="14" t="s">
         <v>3</v>
       </c>
       <c r="R2" s="8" t="s">
         <v>38</v>
       </c>
-      <c r="S2" s="36" t="s">
+      <c r="S2" s="49" t="s">
         <v>37</v>
       </c>
-      <c r="T2" s="37"/>
-      <c r="U2" s="37"/>
-      <c r="V2" s="38"/>
-    </row>
-    <row r="3" spans="1:22" ht="43.2" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A3" s="34" t="s">
+      <c r="T2" s="50"/>
+      <c r="U2" s="50"/>
+      <c r="V2" s="51"/>
+    </row>
+    <row r="3" spans="1:23" ht="43.2" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A3" s="55" t="s">
         <v>21</v>
       </c>
-      <c r="B3" s="34" t="s">
+      <c r="B3" s="55" t="s">
         <v>15</v>
       </c>
       <c r="C3" s="13" t="s">
         <v>5</v>
       </c>
-      <c r="D3" s="24" t="s">
+      <c r="D3" s="63" t="s">
         <v>52</v>
       </c>
-      <c r="E3" s="24"/>
-      <c r="F3" s="24"/>
-      <c r="G3" s="24"/>
-      <c r="H3" s="24"/>
-      <c r="I3" s="24"/>
-      <c r="J3" s="24"/>
-      <c r="K3" s="24"/>
-      <c r="L3" s="24"/>
-      <c r="M3" s="24"/>
-      <c r="N3" s="24"/>
-      <c r="O3" s="24"/>
-      <c r="P3" s="24"/>
-      <c r="Q3" s="25" t="s">
+      <c r="E3" s="63"/>
+      <c r="F3" s="63"/>
+      <c r="G3" s="63"/>
+      <c r="H3" s="63"/>
+      <c r="I3" s="63"/>
+      <c r="J3" s="63"/>
+      <c r="K3" s="63"/>
+      <c r="L3" s="63"/>
+      <c r="M3" s="63"/>
+      <c r="N3" s="63"/>
+      <c r="O3" s="63"/>
+      <c r="P3" s="63"/>
+      <c r="Q3" s="64" t="s">
         <v>53</v>
       </c>
-      <c r="R3" s="41"/>
-      <c r="S3" s="39" t="s">
+      <c r="R3" s="27"/>
+      <c r="S3" s="52" t="s">
         <v>60</v>
       </c>
-      <c r="T3" s="40"/>
-      <c r="U3" s="40"/>
-      <c r="V3" s="41"/>
-    </row>
-    <row r="4" spans="1:22" ht="43.2" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A4" s="35"/>
-      <c r="B4" s="35"/>
-      <c r="C4" s="13" t="s">
+      <c r="T3" s="53"/>
+      <c r="U3" s="53"/>
+      <c r="V3" s="27"/>
+    </row>
+    <row r="4" spans="1:23" ht="43.2" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A4" s="56"/>
+      <c r="B4" s="56"/>
+      <c r="C4" s="70" t="s">
         <v>6</v>
       </c>
-      <c r="D4" s="24"/>
-      <c r="E4" s="24"/>
-      <c r="F4" s="24"/>
-      <c r="G4" s="24"/>
-      <c r="H4" s="24"/>
-      <c r="I4" s="24"/>
-      <c r="J4" s="24"/>
-      <c r="K4" s="24"/>
-      <c r="L4" s="24"/>
-      <c r="M4" s="24"/>
-      <c r="N4" s="24"/>
-      <c r="O4" s="24"/>
-      <c r="P4" s="24"/>
-      <c r="Q4" s="26"/>
-      <c r="R4" s="44"/>
-      <c r="S4" s="42"/>
-      <c r="T4" s="43"/>
-      <c r="U4" s="43"/>
-      <c r="V4" s="44"/>
-    </row>
-    <row r="5" spans="1:22" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A5" s="30" t="s">
+      <c r="D4" s="71"/>
+      <c r="E4" s="71"/>
+      <c r="F4" s="71"/>
+      <c r="G4" s="71"/>
+      <c r="H4" s="71"/>
+      <c r="I4" s="71"/>
+      <c r="J4" s="71"/>
+      <c r="K4" s="71"/>
+      <c r="L4" s="71"/>
+      <c r="M4" s="71"/>
+      <c r="N4" s="71"/>
+      <c r="O4" s="71"/>
+      <c r="P4" s="71"/>
+      <c r="Q4" s="72"/>
+      <c r="R4" s="73"/>
+      <c r="S4" s="74"/>
+      <c r="T4" s="75"/>
+      <c r="U4" s="75"/>
+      <c r="V4" s="73"/>
+    </row>
+    <row r="5" spans="1:23" ht="24" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A5" s="19" t="s">
         <v>29</v>
       </c>
-      <c r="B5" s="31" t="s">
+      <c r="B5" s="68" t="s">
+        <v>62</v>
+      </c>
+      <c r="C5" s="77" t="s">
+        <v>63</v>
+      </c>
+      <c r="D5" s="77"/>
+      <c r="E5" s="77"/>
+      <c r="F5" s="77"/>
+      <c r="G5" s="77"/>
+      <c r="H5" s="77"/>
+      <c r="I5" s="77"/>
+      <c r="J5" s="77"/>
+      <c r="K5" s="77"/>
+      <c r="L5" s="77"/>
+      <c r="M5" s="77"/>
+      <c r="N5" s="77"/>
+      <c r="O5" s="77"/>
+      <c r="P5" s="77"/>
+      <c r="Q5" s="77"/>
+      <c r="R5" s="77"/>
+      <c r="S5" s="77"/>
+      <c r="T5" s="77"/>
+      <c r="U5" s="77"/>
+      <c r="V5" s="77"/>
+      <c r="W5" s="69"/>
+    </row>
+    <row r="6" spans="1:23" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A6" s="54"/>
+      <c r="B6" s="19" t="s">
         <v>15</v>
       </c>
-      <c r="C5" s="1" t="s">
+      <c r="C6" s="76" t="s">
         <v>16</v>
       </c>
-      <c r="D5" s="27" t="s">
+      <c r="D6" s="65" t="s">
         <v>31</v>
       </c>
-      <c r="E5" s="28"/>
-      <c r="F5" s="28"/>
-      <c r="G5" s="28"/>
-      <c r="H5" s="28"/>
-      <c r="I5" s="28"/>
-      <c r="J5" s="28"/>
-      <c r="K5" s="28"/>
-      <c r="L5" s="28"/>
-      <c r="M5" s="28"/>
-      <c r="N5" s="28"/>
-      <c r="O5" s="28"/>
-      <c r="P5" s="29"/>
-      <c r="Q5" s="7" t="s">
+      <c r="E6" s="66"/>
+      <c r="F6" s="66"/>
+      <c r="G6" s="66"/>
+      <c r="H6" s="66"/>
+      <c r="I6" s="66"/>
+      <c r="J6" s="66"/>
+      <c r="K6" s="66"/>
+      <c r="L6" s="66"/>
+      <c r="M6" s="66"/>
+      <c r="N6" s="66"/>
+      <c r="O6" s="66"/>
+      <c r="P6" s="67"/>
+      <c r="Q6" s="7" t="s">
         <v>33</v>
       </c>
-      <c r="R5" s="51" t="s">
+      <c r="R6" s="28" t="s">
         <v>39</v>
       </c>
-      <c r="S5" s="45" t="s">
+      <c r="S6" s="36" t="s">
         <v>40</v>
       </c>
-      <c r="T5" s="46"/>
-      <c r="U5" s="46"/>
-      <c r="V5" s="47"/>
-    </row>
-    <row r="6" spans="1:22" x14ac:dyDescent="0.4">
-      <c r="A6" s="30"/>
-      <c r="B6" s="32"/>
-      <c r="C6" s="1" t="s">
+      <c r="T6" s="37"/>
+      <c r="U6" s="37"/>
+      <c r="V6" s="38"/>
+    </row>
+    <row r="7" spans="1:23" x14ac:dyDescent="0.4">
+      <c r="A7" s="54"/>
+      <c r="B7" s="54"/>
+      <c r="C7" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="D6" s="21" t="s">
+      <c r="D7" s="21" t="s">
         <v>32</v>
-      </c>
-      <c r="E6" s="22"/>
-      <c r="F6" s="22"/>
-      <c r="G6" s="22"/>
-      <c r="H6" s="22"/>
-      <c r="I6" s="22"/>
-      <c r="J6" s="22"/>
-      <c r="K6" s="22"/>
-      <c r="L6" s="22"/>
-      <c r="M6" s="22"/>
-      <c r="N6" s="22"/>
-      <c r="O6" s="22"/>
-      <c r="P6" s="23"/>
-      <c r="Q6" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="R6" s="52"/>
-      <c r="S6" s="45" t="s">
-        <v>42</v>
-      </c>
-      <c r="T6" s="46"/>
-      <c r="U6" s="46"/>
-      <c r="V6" s="47"/>
-    </row>
-    <row r="7" spans="1:22" x14ac:dyDescent="0.4">
-      <c r="A7" s="30"/>
-      <c r="B7" s="32"/>
-      <c r="C7" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="D7" s="21" t="s">
-        <v>31</v>
       </c>
       <c r="E7" s="22"/>
       <c r="F7" s="22"/>
@@ -1959,21 +2343,21 @@
       <c r="O7" s="22"/>
       <c r="P7" s="23"/>
       <c r="Q7" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="R7" s="52"/>
-      <c r="S7" s="45" t="s">
-        <v>40</v>
-      </c>
-      <c r="T7" s="46"/>
-      <c r="U7" s="46"/>
-      <c r="V7" s="47"/>
-    </row>
-    <row r="8" spans="1:22" x14ac:dyDescent="0.4">
-      <c r="A8" s="30"/>
-      <c r="B8" s="32"/>
+        <v>36</v>
+      </c>
+      <c r="R7" s="28"/>
+      <c r="S7" s="39" t="s">
+        <v>42</v>
+      </c>
+      <c r="T7" s="40"/>
+      <c r="U7" s="40"/>
+      <c r="V7" s="41"/>
+    </row>
+    <row r="8" spans="1:23" x14ac:dyDescent="0.4">
+      <c r="A8" s="54"/>
+      <c r="B8" s="54"/>
       <c r="C8" s="1" t="s">
-        <v>25</v>
+        <v>18</v>
       </c>
       <c r="D8" s="21" t="s">
         <v>31</v>
@@ -1991,24 +2375,24 @@
       <c r="O8" s="22"/>
       <c r="P8" s="23"/>
       <c r="Q8" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="R8" s="52"/>
-      <c r="S8" s="45" t="s">
+        <v>34</v>
+      </c>
+      <c r="R8" s="28"/>
+      <c r="S8" s="39" t="s">
         <v>40</v>
       </c>
-      <c r="T8" s="46"/>
-      <c r="U8" s="46"/>
-      <c r="V8" s="47"/>
-    </row>
-    <row r="9" spans="1:22" x14ac:dyDescent="0.4">
-      <c r="A9" s="30"/>
-      <c r="B9" s="32"/>
+      <c r="T8" s="40"/>
+      <c r="U8" s="40"/>
+      <c r="V8" s="41"/>
+    </row>
+    <row r="9" spans="1:23" x14ac:dyDescent="0.4">
+      <c r="A9" s="54"/>
+      <c r="B9" s="54"/>
       <c r="C9" s="1" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="D9" s="21" t="s">
-        <v>41</v>
+        <v>31</v>
       </c>
       <c r="E9" s="22"/>
       <c r="F9" s="22"/>
@@ -2023,21 +2407,21 @@
       <c r="O9" s="22"/>
       <c r="P9" s="23"/>
       <c r="Q9" s="3" t="s">
-        <v>44</v>
-      </c>
-      <c r="R9" s="52"/>
-      <c r="S9" s="54" t="s">
-        <v>51</v>
-      </c>
-      <c r="T9" s="55"/>
-      <c r="U9" s="55"/>
-      <c r="V9" s="56"/>
-    </row>
-    <row r="10" spans="1:22" x14ac:dyDescent="0.4">
-      <c r="A10" s="30"/>
-      <c r="B10" s="32"/>
+        <v>35</v>
+      </c>
+      <c r="R9" s="28"/>
+      <c r="S9" s="39" t="s">
+        <v>40</v>
+      </c>
+      <c r="T9" s="40"/>
+      <c r="U9" s="40"/>
+      <c r="V9" s="41"/>
+    </row>
+    <row r="10" spans="1:23" x14ac:dyDescent="0.4">
+      <c r="A10" s="54"/>
+      <c r="B10" s="54"/>
       <c r="C10" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D10" s="21" t="s">
         <v>41</v>
@@ -2055,22 +2439,24 @@
       <c r="O10" s="22"/>
       <c r="P10" s="23"/>
       <c r="Q10" s="3" t="s">
-        <v>45</v>
-      </c>
-      <c r="R10" s="52"/>
-      <c r="S10" s="57"/>
-      <c r="T10" s="58"/>
-      <c r="U10" s="58"/>
-      <c r="V10" s="59"/>
-    </row>
-    <row r="11" spans="1:22" x14ac:dyDescent="0.4">
-      <c r="A11" s="30"/>
-      <c r="B11" s="32"/>
+        <v>44</v>
+      </c>
+      <c r="R10" s="28"/>
+      <c r="S10" s="30" t="s">
+        <v>51</v>
+      </c>
+      <c r="T10" s="31"/>
+      <c r="U10" s="31"/>
+      <c r="V10" s="32"/>
+    </row>
+    <row r="11" spans="1:23" x14ac:dyDescent="0.4">
+      <c r="A11" s="54"/>
+      <c r="B11" s="54"/>
       <c r="C11" s="1" t="s">
-        <v>22</v>
+        <v>28</v>
       </c>
       <c r="D11" s="21" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="E11" s="22"/>
       <c r="F11" s="22"/>
@@ -2085,19 +2471,19 @@
       <c r="O11" s="22"/>
       <c r="P11" s="23"/>
       <c r="Q11" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="R11" s="52"/>
-      <c r="S11" s="57"/>
-      <c r="T11" s="58"/>
-      <c r="U11" s="58"/>
-      <c r="V11" s="59"/>
-    </row>
-    <row r="12" spans="1:22" x14ac:dyDescent="0.4">
-      <c r="A12" s="30"/>
-      <c r="B12" s="32"/>
+        <v>45</v>
+      </c>
+      <c r="R11" s="28"/>
+      <c r="S11" s="33"/>
+      <c r="T11" s="34"/>
+      <c r="U11" s="34"/>
+      <c r="V11" s="35"/>
+    </row>
+    <row r="12" spans="1:23" x14ac:dyDescent="0.4">
+      <c r="A12" s="54"/>
+      <c r="B12" s="54"/>
       <c r="C12" s="1" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="D12" s="21" t="s">
         <v>43</v>
@@ -2115,19 +2501,19 @@
       <c r="O12" s="22"/>
       <c r="P12" s="23"/>
       <c r="Q12" s="3" t="s">
-        <v>46</v>
-      </c>
-      <c r="R12" s="52"/>
-      <c r="S12" s="57"/>
-      <c r="T12" s="58"/>
-      <c r="U12" s="58"/>
-      <c r="V12" s="59"/>
-    </row>
-    <row r="13" spans="1:22" x14ac:dyDescent="0.4">
-      <c r="A13" s="30"/>
-      <c r="B13" s="32"/>
+        <v>36</v>
+      </c>
+      <c r="R12" s="28"/>
+      <c r="S12" s="33"/>
+      <c r="T12" s="34"/>
+      <c r="U12" s="34"/>
+      <c r="V12" s="35"/>
+    </row>
+    <row r="13" spans="1:23" x14ac:dyDescent="0.4">
+      <c r="A13" s="54"/>
+      <c r="B13" s="54"/>
       <c r="C13" s="1" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="D13" s="21" t="s">
         <v>43</v>
@@ -2145,19 +2531,19 @@
       <c r="O13" s="22"/>
       <c r="P13" s="23"/>
       <c r="Q13" s="3" t="s">
-        <v>49</v>
-      </c>
-      <c r="R13" s="52"/>
-      <c r="S13" s="57"/>
-      <c r="T13" s="58"/>
-      <c r="U13" s="58"/>
-      <c r="V13" s="59"/>
-    </row>
-    <row r="14" spans="1:22" x14ac:dyDescent="0.4">
-      <c r="A14" s="30"/>
-      <c r="B14" s="32"/>
+        <v>46</v>
+      </c>
+      <c r="R13" s="28"/>
+      <c r="S13" s="33"/>
+      <c r="T13" s="34"/>
+      <c r="U13" s="34"/>
+      <c r="V13" s="35"/>
+    </row>
+    <row r="14" spans="1:23" x14ac:dyDescent="0.4">
+      <c r="A14" s="54"/>
+      <c r="B14" s="54"/>
       <c r="C14" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D14" s="21" t="s">
         <v>43</v>
@@ -2175,22 +2561,22 @@
       <c r="O14" s="22"/>
       <c r="P14" s="23"/>
       <c r="Q14" s="3" t="s">
-        <v>50</v>
-      </c>
-      <c r="R14" s="52"/>
-      <c r="S14" s="57"/>
-      <c r="T14" s="58"/>
-      <c r="U14" s="58"/>
-      <c r="V14" s="59"/>
-    </row>
-    <row r="15" spans="1:22" x14ac:dyDescent="0.4">
-      <c r="A15" s="30"/>
-      <c r="B15" s="32"/>
+        <v>49</v>
+      </c>
+      <c r="R14" s="28"/>
+      <c r="S14" s="33"/>
+      <c r="T14" s="34"/>
+      <c r="U14" s="34"/>
+      <c r="V14" s="35"/>
+    </row>
+    <row r="15" spans="1:23" x14ac:dyDescent="0.4">
+      <c r="A15" s="54"/>
+      <c r="B15" s="54"/>
       <c r="C15" s="1" t="s">
-        <v>19</v>
+        <v>24</v>
       </c>
       <c r="D15" s="21" t="s">
-        <v>43</v>
+        <v>67</v>
       </c>
       <c r="E15" s="22"/>
       <c r="F15" s="22"/>
@@ -2205,19 +2591,19 @@
       <c r="O15" s="22"/>
       <c r="P15" s="23"/>
       <c r="Q15" s="3" t="s">
-        <v>47</v>
-      </c>
-      <c r="R15" s="52"/>
-      <c r="S15" s="57"/>
-      <c r="T15" s="58"/>
-      <c r="U15" s="58"/>
-      <c r="V15" s="59"/>
-    </row>
-    <row r="16" spans="1:22" x14ac:dyDescent="0.4">
-      <c r="A16" s="30"/>
-      <c r="B16" s="32"/>
+        <v>50</v>
+      </c>
+      <c r="R15" s="28"/>
+      <c r="S15" s="33"/>
+      <c r="T15" s="34"/>
+      <c r="U15" s="34"/>
+      <c r="V15" s="35"/>
+    </row>
+    <row r="16" spans="1:23" x14ac:dyDescent="0.4">
+      <c r="A16" s="54"/>
+      <c r="B16" s="54"/>
       <c r="C16" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D16" s="21" t="s">
         <v>43</v>
@@ -2235,22 +2621,22 @@
       <c r="O16" s="22"/>
       <c r="P16" s="23"/>
       <c r="Q16" s="3" t="s">
-        <v>48</v>
-      </c>
-      <c r="R16" s="53"/>
-      <c r="S16" s="60"/>
-      <c r="T16" s="61"/>
-      <c r="U16" s="61"/>
-      <c r="V16" s="62"/>
-    </row>
-    <row r="17" spans="1:22" ht="34.799999999999997" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A17" s="30"/>
-      <c r="B17" s="32"/>
+        <v>47</v>
+      </c>
+      <c r="R16" s="28"/>
+      <c r="S16" s="33"/>
+      <c r="T16" s="34"/>
+      <c r="U16" s="34"/>
+      <c r="V16" s="35"/>
+    </row>
+    <row r="17" spans="1:23" x14ac:dyDescent="0.4">
+      <c r="A17" s="54"/>
+      <c r="B17" s="54"/>
       <c r="C17" s="1" t="s">
-        <v>7</v>
+        <v>20</v>
       </c>
       <c r="D17" s="21" t="s">
-        <v>57</v>
+        <v>43</v>
       </c>
       <c r="E17" s="22"/>
       <c r="F17" s="22"/>
@@ -2264,22 +2650,20 @@
       <c r="N17" s="22"/>
       <c r="O17" s="22"/>
       <c r="P17" s="23"/>
-      <c r="Q17" s="12" t="s">
-        <v>58</v>
-      </c>
-      <c r="R17" s="31"/>
-      <c r="S17" s="66" t="s">
-        <v>61</v>
-      </c>
-      <c r="T17" s="67"/>
-      <c r="U17" s="67"/>
-      <c r="V17" s="68"/>
-    </row>
-    <row r="18" spans="1:22" ht="34.799999999999997" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A18" s="30"/>
-      <c r="B18" s="32"/>
+      <c r="Q17" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="R17" s="29"/>
+      <c r="S17" s="36"/>
+      <c r="T17" s="37"/>
+      <c r="U17" s="37"/>
+      <c r="V17" s="38"/>
+    </row>
+    <row r="18" spans="1:23" ht="34.799999999999997" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A18" s="54"/>
+      <c r="B18" s="54"/>
       <c r="C18" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D18" s="21" t="s">
         <v>57</v>
@@ -2297,21 +2681,25 @@
       <c r="O18" s="22"/>
       <c r="P18" s="23"/>
       <c r="Q18" s="12" t="s">
-        <v>59</v>
-      </c>
-      <c r="R18" s="33"/>
-      <c r="S18" s="69"/>
-      <c r="T18" s="70"/>
-      <c r="U18" s="70"/>
-      <c r="V18" s="71"/>
-    </row>
-    <row r="19" spans="1:22" ht="15.6" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A19" s="30"/>
-      <c r="B19" s="32"/>
+        <v>58</v>
+      </c>
+      <c r="R18" s="19"/>
+      <c r="S18" s="43" t="s">
+        <v>61</v>
+      </c>
+      <c r="T18" s="44"/>
+      <c r="U18" s="44"/>
+      <c r="V18" s="45"/>
+    </row>
+    <row r="19" spans="1:23" ht="34.799999999999997" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A19" s="54"/>
+      <c r="B19" s="54"/>
       <c r="C19" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="D19" s="21"/>
+        <v>8</v>
+      </c>
+      <c r="D19" s="21" t="s">
+        <v>57</v>
+      </c>
       <c r="E19" s="22"/>
       <c r="F19" s="22"/>
       <c r="G19" s="22"/>
@@ -2324,21 +2712,23 @@
       <c r="N19" s="22"/>
       <c r="O19" s="22"/>
       <c r="P19" s="23"/>
-      <c r="Q19" s="12"/>
-      <c r="R19" s="11"/>
-      <c r="S19" s="21"/>
-      <c r="T19" s="22"/>
-      <c r="U19" s="22"/>
-      <c r="V19" s="23"/>
-    </row>
-    <row r="20" spans="1:22" ht="52.2" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A20" s="30"/>
-      <c r="B20" s="33"/>
+      <c r="Q19" s="12" t="s">
+        <v>59</v>
+      </c>
+      <c r="R19" s="20"/>
+      <c r="S19" s="46"/>
+      <c r="T19" s="47"/>
+      <c r="U19" s="47"/>
+      <c r="V19" s="48"/>
+    </row>
+    <row r="20" spans="1:23" ht="15.6" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A20" s="54"/>
+      <c r="B20" s="54"/>
       <c r="C20" s="1" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="D20" s="21" t="s">
-        <v>54</v>
+        <v>64</v>
       </c>
       <c r="E20" s="22"/>
       <c r="F20" s="22"/>
@@ -2352,26 +2742,26 @@
       <c r="N20" s="22"/>
       <c r="O20" s="22"/>
       <c r="P20" s="23"/>
-      <c r="Q20" s="63" t="s">
-        <v>55</v>
-      </c>
-      <c r="R20" s="64"/>
-      <c r="S20" s="65" t="s">
-        <v>56</v>
-      </c>
-      <c r="T20" s="46"/>
-      <c r="U20" s="46"/>
-      <c r="V20" s="47"/>
-    </row>
-    <row r="21" spans="1:22" x14ac:dyDescent="0.4">
-      <c r="A21" s="30"/>
-      <c r="B21" s="31" t="s">
-        <v>30</v>
-      </c>
+      <c r="Q20" s="15" t="s">
+        <v>65</v>
+      </c>
+      <c r="R20" s="11"/>
+      <c r="S20" s="21" t="s">
+        <v>66</v>
+      </c>
+      <c r="T20" s="22"/>
+      <c r="U20" s="22"/>
+      <c r="V20" s="23"/>
+    </row>
+    <row r="21" spans="1:23" ht="52.2" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A21" s="54"/>
+      <c r="B21" s="20"/>
       <c r="C21" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="D21" s="21"/>
+        <v>13</v>
+      </c>
+      <c r="D21" s="21" t="s">
+        <v>54</v>
+      </c>
       <c r="E21" s="22"/>
       <c r="F21" s="22"/>
       <c r="G21" s="22"/>
@@ -2384,20 +2774,28 @@
       <c r="N21" s="22"/>
       <c r="O21" s="22"/>
       <c r="P21" s="23"/>
-      <c r="Q21" s="3"/>
-      <c r="R21" s="10"/>
-      <c r="S21" s="45"/>
-      <c r="T21" s="46"/>
-      <c r="U21" s="46"/>
-      <c r="V21" s="47"/>
-    </row>
-    <row r="22" spans="1:22" x14ac:dyDescent="0.4">
-      <c r="A22" s="30"/>
-      <c r="B22" s="32"/>
+      <c r="Q21" s="17" t="s">
+        <v>55</v>
+      </c>
+      <c r="R21" s="18"/>
+      <c r="S21" s="42" t="s">
+        <v>56</v>
+      </c>
+      <c r="T21" s="40"/>
+      <c r="U21" s="40"/>
+      <c r="V21" s="41"/>
+    </row>
+    <row r="22" spans="1:23" x14ac:dyDescent="0.4">
+      <c r="A22" s="54"/>
+      <c r="B22" s="19" t="s">
+        <v>30</v>
+      </c>
       <c r="C22" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="D22" s="21"/>
+        <v>10</v>
+      </c>
+      <c r="D22" s="21" t="s">
+        <v>69</v>
+      </c>
       <c r="E22" s="22"/>
       <c r="F22" s="22"/>
       <c r="G22" s="22"/>
@@ -2412,18 +2810,22 @@
       <c r="P22" s="23"/>
       <c r="Q22" s="3"/>
       <c r="R22" s="10"/>
-      <c r="S22" s="45"/>
-      <c r="T22" s="46"/>
-      <c r="U22" s="46"/>
-      <c r="V22" s="47"/>
-    </row>
-    <row r="23" spans="1:22" x14ac:dyDescent="0.4">
-      <c r="A23" s="30"/>
-      <c r="B23" s="32"/>
+      <c r="S22" s="43" t="s">
+        <v>70</v>
+      </c>
+      <c r="T22" s="44"/>
+      <c r="U22" s="44"/>
+      <c r="V22" s="45"/>
+    </row>
+    <row r="23" spans="1:23" x14ac:dyDescent="0.4">
+      <c r="A23" s="54"/>
+      <c r="B23" s="54"/>
       <c r="C23" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="D23" s="21"/>
+        <v>11</v>
+      </c>
+      <c r="D23" s="21" t="s">
+        <v>71</v>
+      </c>
       <c r="E23" s="22"/>
       <c r="F23" s="22"/>
       <c r="G23" s="22"/>
@@ -2438,16 +2840,20 @@
       <c r="P23" s="23"/>
       <c r="Q23" s="3"/>
       <c r="R23" s="10"/>
-      <c r="S23" s="45"/>
-      <c r="T23" s="46"/>
-      <c r="U23" s="46"/>
-      <c r="V23" s="47"/>
-    </row>
-    <row r="24" spans="1:22" x14ac:dyDescent="0.4">
-      <c r="A24" s="30"/>
-      <c r="B24" s="32"/>
-      <c r="C24" s="1"/>
-      <c r="D24" s="21"/>
+      <c r="S23" s="78"/>
+      <c r="T23" s="79"/>
+      <c r="U23" s="79"/>
+      <c r="V23" s="80"/>
+    </row>
+    <row r="24" spans="1:23" x14ac:dyDescent="0.4">
+      <c r="A24" s="54"/>
+      <c r="B24" s="54"/>
+      <c r="C24" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D24" s="21" t="s">
+        <v>71</v>
+      </c>
       <c r="E24" s="22"/>
       <c r="F24" s="22"/>
       <c r="G24" s="22"/>
@@ -2462,373 +2868,410 @@
       <c r="P24" s="23"/>
       <c r="Q24" s="3"/>
       <c r="R24" s="10"/>
-      <c r="S24" s="45"/>
-      <c r="T24" s="46"/>
-      <c r="U24" s="46"/>
-      <c r="V24" s="47"/>
-    </row>
-    <row r="25" spans="1:22" x14ac:dyDescent="0.4">
-      <c r="A25" s="30"/>
-      <c r="B25" s="32"/>
-      <c r="C25" s="1"/>
-      <c r="D25" s="21"/>
-      <c r="E25" s="22"/>
-      <c r="F25" s="22"/>
-      <c r="G25" s="22"/>
-      <c r="H25" s="22"/>
-      <c r="I25" s="22"/>
-      <c r="J25" s="22"/>
-      <c r="K25" s="22"/>
-      <c r="L25" s="22"/>
-      <c r="M25" s="22"/>
-      <c r="N25" s="22"/>
-      <c r="O25" s="22"/>
-      <c r="P25" s="23"/>
-      <c r="Q25" s="3"/>
-      <c r="R25" s="10"/>
-      <c r="S25" s="45"/>
-      <c r="T25" s="46"/>
-      <c r="U25" s="46"/>
-      <c r="V25" s="47"/>
-    </row>
-    <row r="26" spans="1:22" x14ac:dyDescent="0.4">
-      <c r="A26" s="30"/>
-      <c r="B26" s="32"/>
-      <c r="C26" s="1"/>
-      <c r="D26" s="21"/>
-      <c r="E26" s="22"/>
-      <c r="F26" s="22"/>
-      <c r="G26" s="22"/>
-      <c r="H26" s="22"/>
-      <c r="I26" s="22"/>
-      <c r="J26" s="22"/>
-      <c r="K26" s="22"/>
-      <c r="L26" s="22"/>
-      <c r="M26" s="22"/>
-      <c r="N26" s="22"/>
-      <c r="O26" s="22"/>
-      <c r="P26" s="23"/>
-      <c r="Q26" s="3"/>
-      <c r="R26" s="10"/>
-      <c r="S26" s="45"/>
-      <c r="T26" s="46"/>
-      <c r="U26" s="46"/>
-      <c r="V26" s="47"/>
-    </row>
-    <row r="27" spans="1:22" x14ac:dyDescent="0.4">
-      <c r="A27" s="30"/>
-      <c r="B27" s="32"/>
-      <c r="C27" s="1"/>
-      <c r="D27" s="21"/>
-      <c r="E27" s="22"/>
-      <c r="F27" s="22"/>
-      <c r="G27" s="22"/>
-      <c r="H27" s="22"/>
-      <c r="I27" s="22"/>
-      <c r="J27" s="22"/>
-      <c r="K27" s="22"/>
-      <c r="L27" s="22"/>
-      <c r="M27" s="22"/>
-      <c r="N27" s="22"/>
-      <c r="O27" s="22"/>
-      <c r="P27" s="23"/>
-      <c r="Q27" s="3"/>
-      <c r="R27" s="10"/>
-      <c r="S27" s="45"/>
-      <c r="T27" s="46"/>
-      <c r="U27" s="46"/>
-      <c r="V27" s="47"/>
-    </row>
-    <row r="28" spans="1:22" x14ac:dyDescent="0.4">
-      <c r="A28" s="30"/>
-      <c r="B28" s="32"/>
-      <c r="C28" s="1"/>
-      <c r="D28" s="21"/>
-      <c r="E28" s="22"/>
-      <c r="F28" s="22"/>
-      <c r="G28" s="22"/>
-      <c r="H28" s="22"/>
-      <c r="I28" s="22"/>
-      <c r="J28" s="22"/>
-      <c r="K28" s="22"/>
-      <c r="L28" s="22"/>
-      <c r="M28" s="22"/>
-      <c r="N28" s="22"/>
-      <c r="O28" s="22"/>
-      <c r="P28" s="23"/>
-      <c r="Q28" s="3"/>
-      <c r="R28" s="10"/>
-      <c r="S28" s="45"/>
-      <c r="T28" s="46"/>
-      <c r="U28" s="46"/>
-      <c r="V28" s="47"/>
-    </row>
-    <row r="29" spans="1:22" x14ac:dyDescent="0.4">
-      <c r="A29" s="30"/>
-      <c r="B29" s="32"/>
-      <c r="C29" s="1"/>
-      <c r="D29" s="21"/>
-      <c r="E29" s="22"/>
-      <c r="F29" s="22"/>
-      <c r="G29" s="22"/>
-      <c r="H29" s="22"/>
-      <c r="I29" s="22"/>
-      <c r="J29" s="22"/>
-      <c r="K29" s="22"/>
-      <c r="L29" s="22"/>
-      <c r="M29" s="22"/>
-      <c r="N29" s="22"/>
-      <c r="O29" s="22"/>
-      <c r="P29" s="23"/>
-      <c r="Q29" s="3"/>
-      <c r="R29" s="10"/>
-      <c r="S29" s="45"/>
-      <c r="T29" s="46"/>
-      <c r="U29" s="46"/>
-      <c r="V29" s="47"/>
-    </row>
-    <row r="30" spans="1:22" x14ac:dyDescent="0.4">
-      <c r="A30" s="30"/>
-      <c r="B30" s="32"/>
-      <c r="C30" s="1"/>
-      <c r="D30" s="21"/>
-      <c r="E30" s="22"/>
-      <c r="F30" s="22"/>
-      <c r="G30" s="22"/>
-      <c r="H30" s="22"/>
-      <c r="I30" s="22"/>
-      <c r="J30" s="22"/>
-      <c r="K30" s="22"/>
-      <c r="L30" s="22"/>
-      <c r="M30" s="22"/>
-      <c r="N30" s="22"/>
-      <c r="O30" s="22"/>
-      <c r="P30" s="23"/>
-      <c r="Q30" s="3"/>
-      <c r="R30" s="10"/>
-      <c r="S30" s="45"/>
-      <c r="T30" s="46"/>
-      <c r="U30" s="46"/>
-      <c r="V30" s="47"/>
-    </row>
-    <row r="31" spans="1:22" x14ac:dyDescent="0.4">
-      <c r="A31" s="30"/>
-      <c r="B31" s="32"/>
-      <c r="C31" s="1"/>
-      <c r="D31" s="21"/>
-      <c r="E31" s="22"/>
-      <c r="F31" s="22"/>
-      <c r="G31" s="22"/>
-      <c r="H31" s="22"/>
-      <c r="I31" s="22"/>
-      <c r="J31" s="22"/>
-      <c r="K31" s="22"/>
-      <c r="L31" s="22"/>
-      <c r="M31" s="22"/>
-      <c r="N31" s="22"/>
-      <c r="O31" s="22"/>
-      <c r="P31" s="23"/>
-      <c r="Q31" s="3"/>
-      <c r="R31" s="10"/>
-      <c r="S31" s="45"/>
-      <c r="T31" s="46"/>
-      <c r="U31" s="46"/>
-      <c r="V31" s="47"/>
-    </row>
-    <row r="32" spans="1:22" x14ac:dyDescent="0.4">
-      <c r="A32" s="30"/>
-      <c r="B32" s="32"/>
-      <c r="C32" s="1"/>
-      <c r="D32" s="21"/>
-      <c r="E32" s="22"/>
-      <c r="F32" s="22"/>
-      <c r="G32" s="22"/>
-      <c r="H32" s="22"/>
-      <c r="I32" s="22"/>
-      <c r="J32" s="22"/>
-      <c r="K32" s="22"/>
-      <c r="L32" s="22"/>
-      <c r="M32" s="22"/>
-      <c r="N32" s="22"/>
-      <c r="O32" s="22"/>
-      <c r="P32" s="23"/>
-      <c r="Q32" s="3"/>
-      <c r="R32" s="10"/>
-      <c r="S32" s="45"/>
-      <c r="T32" s="46"/>
-      <c r="U32" s="46"/>
-      <c r="V32" s="47"/>
-    </row>
-    <row r="33" spans="1:22" x14ac:dyDescent="0.4">
-      <c r="A33" s="30"/>
-      <c r="B33" s="33"/>
-      <c r="C33" s="1"/>
-      <c r="D33" s="21"/>
-      <c r="E33" s="22"/>
-      <c r="F33" s="22"/>
-      <c r="G33" s="22"/>
-      <c r="H33" s="22"/>
-      <c r="I33" s="22"/>
-      <c r="J33" s="22"/>
-      <c r="K33" s="22"/>
-      <c r="L33" s="22"/>
-      <c r="M33" s="22"/>
-      <c r="N33" s="22"/>
-      <c r="O33" s="22"/>
-      <c r="P33" s="23"/>
-      <c r="Q33" s="3"/>
-      <c r="R33" s="10"/>
-      <c r="S33" s="45"/>
-      <c r="T33" s="46"/>
-      <c r="U33" s="46"/>
-      <c r="V33" s="47"/>
-    </row>
-    <row r="34" spans="1:22" x14ac:dyDescent="0.4">
-      <c r="A34" s="30"/>
-      <c r="B34" s="3"/>
-      <c r="C34" s="1"/>
-      <c r="D34" s="21"/>
-      <c r="E34" s="22"/>
-      <c r="F34" s="22"/>
-      <c r="G34" s="22"/>
-      <c r="H34" s="22"/>
-      <c r="I34" s="22"/>
-      <c r="J34" s="22"/>
-      <c r="K34" s="22"/>
-      <c r="L34" s="22"/>
-      <c r="M34" s="22"/>
-      <c r="N34" s="22"/>
-      <c r="O34" s="22"/>
-      <c r="P34" s="23"/>
-      <c r="Q34" s="3"/>
-      <c r="R34" s="10"/>
-      <c r="S34" s="45"/>
-      <c r="T34" s="46"/>
-      <c r="U34" s="46"/>
-      <c r="V34" s="47"/>
-    </row>
-    <row r="35" spans="1:22" x14ac:dyDescent="0.4">
-      <c r="A35" s="30"/>
-      <c r="B35" s="3"/>
-      <c r="C35" s="1"/>
-      <c r="D35" s="21"/>
-      <c r="E35" s="22"/>
-      <c r="F35" s="22"/>
-      <c r="G35" s="22"/>
-      <c r="H35" s="22"/>
-      <c r="I35" s="22"/>
-      <c r="J35" s="22"/>
-      <c r="K35" s="22"/>
-      <c r="L35" s="22"/>
-      <c r="M35" s="22"/>
-      <c r="N35" s="22"/>
-      <c r="O35" s="22"/>
-      <c r="P35" s="23"/>
-      <c r="Q35" s="3"/>
-      <c r="R35" s="10"/>
-      <c r="S35" s="45"/>
-      <c r="T35" s="46"/>
-      <c r="U35" s="46"/>
-      <c r="V35" s="47"/>
-    </row>
-    <row r="36" spans="1:22" x14ac:dyDescent="0.4">
-      <c r="A36" s="30"/>
-      <c r="B36" s="3"/>
-      <c r="C36" s="1"/>
-      <c r="D36" s="21"/>
-      <c r="E36" s="22"/>
-      <c r="F36" s="22"/>
-      <c r="G36" s="22"/>
-      <c r="H36" s="22"/>
-      <c r="I36" s="22"/>
-      <c r="J36" s="22"/>
-      <c r="K36" s="22"/>
-      <c r="L36" s="22"/>
-      <c r="M36" s="22"/>
-      <c r="N36" s="22"/>
-      <c r="O36" s="22"/>
-      <c r="P36" s="23"/>
-      <c r="Q36" s="3"/>
-      <c r="R36" s="10"/>
-      <c r="S36" s="45"/>
-      <c r="T36" s="46"/>
-      <c r="U36" s="46"/>
-      <c r="V36" s="47"/>
+      <c r="S24" s="78"/>
+      <c r="T24" s="79"/>
+      <c r="U24" s="79"/>
+      <c r="V24" s="80"/>
+    </row>
+    <row r="25" spans="1:23" ht="63" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A25" s="54"/>
+      <c r="B25" s="54"/>
+      <c r="C25" s="81" t="s">
+        <v>68</v>
+      </c>
+      <c r="D25" s="82" t="s">
+        <v>69</v>
+      </c>
+      <c r="E25" s="83"/>
+      <c r="F25" s="83"/>
+      <c r="G25" s="83"/>
+      <c r="H25" s="83"/>
+      <c r="I25" s="83"/>
+      <c r="J25" s="83"/>
+      <c r="K25" s="83"/>
+      <c r="L25" s="83"/>
+      <c r="M25" s="83"/>
+      <c r="N25" s="83"/>
+      <c r="O25" s="83"/>
+      <c r="P25" s="84"/>
+      <c r="Q25" s="16"/>
+      <c r="R25" s="85"/>
+      <c r="S25" s="78"/>
+      <c r="T25" s="79"/>
+      <c r="U25" s="79"/>
+      <c r="V25" s="80"/>
+    </row>
+    <row r="26" spans="1:23" x14ac:dyDescent="0.4">
+      <c r="A26" s="88"/>
+      <c r="B26" s="88"/>
+      <c r="C26" s="89"/>
+      <c r="D26" s="88"/>
+      <c r="E26" s="88"/>
+      <c r="F26" s="88"/>
+      <c r="G26" s="88"/>
+      <c r="H26" s="88"/>
+      <c r="I26" s="88"/>
+      <c r="J26" s="88"/>
+      <c r="K26" s="88"/>
+      <c r="L26" s="88"/>
+      <c r="M26" s="88"/>
+      <c r="N26" s="88"/>
+      <c r="O26" s="88"/>
+      <c r="P26" s="88"/>
+      <c r="Q26" s="90"/>
+      <c r="R26" s="90"/>
+      <c r="S26" s="88"/>
+      <c r="T26" s="88"/>
+      <c r="U26" s="88"/>
+      <c r="V26" s="88"/>
+      <c r="W26" s="69"/>
+    </row>
+    <row r="27" spans="1:23" x14ac:dyDescent="0.4">
+      <c r="A27" s="88"/>
+      <c r="B27" s="88"/>
+      <c r="C27" s="89"/>
+      <c r="D27" s="88"/>
+      <c r="E27" s="88"/>
+      <c r="F27" s="88"/>
+      <c r="G27" s="88"/>
+      <c r="H27" s="88"/>
+      <c r="I27" s="88"/>
+      <c r="J27" s="88"/>
+      <c r="K27" s="88"/>
+      <c r="L27" s="88"/>
+      <c r="M27" s="88"/>
+      <c r="N27" s="88"/>
+      <c r="O27" s="88"/>
+      <c r="P27" s="88"/>
+      <c r="Q27" s="90"/>
+      <c r="R27" s="90"/>
+      <c r="S27" s="88"/>
+      <c r="T27" s="88"/>
+      <c r="U27" s="88"/>
+      <c r="V27" s="88"/>
+      <c r="W27" s="69"/>
+    </row>
+    <row r="28" spans="1:23" x14ac:dyDescent="0.4">
+      <c r="A28" s="88"/>
+      <c r="B28" s="88"/>
+      <c r="C28" s="89"/>
+      <c r="D28" s="88"/>
+      <c r="E28" s="88"/>
+      <c r="F28" s="88"/>
+      <c r="G28" s="88"/>
+      <c r="H28" s="88"/>
+      <c r="I28" s="88"/>
+      <c r="J28" s="88"/>
+      <c r="K28" s="88"/>
+      <c r="L28" s="88"/>
+      <c r="M28" s="88"/>
+      <c r="N28" s="88"/>
+      <c r="O28" s="88"/>
+      <c r="P28" s="88"/>
+      <c r="Q28" s="90"/>
+      <c r="R28" s="90"/>
+      <c r="S28" s="88"/>
+      <c r="T28" s="88"/>
+      <c r="U28" s="88"/>
+      <c r="V28" s="88"/>
+      <c r="W28" s="69"/>
+    </row>
+    <row r="29" spans="1:23" x14ac:dyDescent="0.4">
+      <c r="A29" s="88"/>
+      <c r="B29" s="88"/>
+      <c r="C29" s="89"/>
+      <c r="D29" s="88"/>
+      <c r="E29" s="88"/>
+      <c r="F29" s="88"/>
+      <c r="G29" s="88"/>
+      <c r="H29" s="88"/>
+      <c r="I29" s="88"/>
+      <c r="J29" s="88"/>
+      <c r="K29" s="88"/>
+      <c r="L29" s="88"/>
+      <c r="M29" s="88"/>
+      <c r="N29" s="88"/>
+      <c r="O29" s="88"/>
+      <c r="P29" s="88"/>
+      <c r="Q29" s="90"/>
+      <c r="R29" s="90"/>
+      <c r="S29" s="88"/>
+      <c r="T29" s="88"/>
+      <c r="U29" s="88"/>
+      <c r="V29" s="88"/>
+      <c r="W29" s="69"/>
+    </row>
+    <row r="30" spans="1:23" x14ac:dyDescent="0.4">
+      <c r="A30" s="88"/>
+      <c r="B30" s="88"/>
+      <c r="C30" s="89"/>
+      <c r="D30" s="88"/>
+      <c r="E30" s="88"/>
+      <c r="F30" s="88"/>
+      <c r="G30" s="88"/>
+      <c r="H30" s="88"/>
+      <c r="I30" s="88"/>
+      <c r="J30" s="88"/>
+      <c r="K30" s="88"/>
+      <c r="L30" s="88"/>
+      <c r="M30" s="88"/>
+      <c r="N30" s="88"/>
+      <c r="O30" s="88"/>
+      <c r="P30" s="88"/>
+      <c r="Q30" s="90"/>
+      <c r="R30" s="90"/>
+      <c r="S30" s="88"/>
+      <c r="T30" s="88"/>
+      <c r="U30" s="88"/>
+      <c r="V30" s="88"/>
+      <c r="W30" s="69"/>
+    </row>
+    <row r="31" spans="1:23" x14ac:dyDescent="0.4">
+      <c r="A31" s="88"/>
+      <c r="B31" s="88"/>
+      <c r="C31" s="89"/>
+      <c r="D31" s="88"/>
+      <c r="E31" s="88"/>
+      <c r="F31" s="88"/>
+      <c r="G31" s="88"/>
+      <c r="H31" s="88"/>
+      <c r="I31" s="88"/>
+      <c r="J31" s="88"/>
+      <c r="K31" s="88"/>
+      <c r="L31" s="88"/>
+      <c r="M31" s="88"/>
+      <c r="N31" s="88"/>
+      <c r="O31" s="88"/>
+      <c r="P31" s="88"/>
+      <c r="Q31" s="90"/>
+      <c r="R31" s="90"/>
+      <c r="S31" s="88"/>
+      <c r="T31" s="88"/>
+      <c r="U31" s="88"/>
+      <c r="V31" s="88"/>
+      <c r="W31" s="69"/>
+    </row>
+    <row r="32" spans="1:23" x14ac:dyDescent="0.4">
+      <c r="A32" s="88"/>
+      <c r="B32" s="88"/>
+      <c r="C32" s="89"/>
+      <c r="D32" s="88"/>
+      <c r="E32" s="88"/>
+      <c r="F32" s="88"/>
+      <c r="G32" s="88"/>
+      <c r="H32" s="88"/>
+      <c r="I32" s="88"/>
+      <c r="J32" s="88"/>
+      <c r="K32" s="88"/>
+      <c r="L32" s="88"/>
+      <c r="M32" s="88"/>
+      <c r="N32" s="88"/>
+      <c r="O32" s="88"/>
+      <c r="P32" s="88"/>
+      <c r="Q32" s="90"/>
+      <c r="R32" s="90"/>
+      <c r="S32" s="88"/>
+      <c r="T32" s="88"/>
+      <c r="U32" s="88"/>
+      <c r="V32" s="88"/>
+      <c r="W32" s="69"/>
+    </row>
+    <row r="33" spans="1:23" x14ac:dyDescent="0.4">
+      <c r="A33" s="88"/>
+      <c r="B33" s="88"/>
+      <c r="C33" s="89"/>
+      <c r="D33" s="88"/>
+      <c r="E33" s="88"/>
+      <c r="F33" s="88"/>
+      <c r="G33" s="88"/>
+      <c r="H33" s="88"/>
+      <c r="I33" s="88"/>
+      <c r="J33" s="88"/>
+      <c r="K33" s="88"/>
+      <c r="L33" s="88"/>
+      <c r="M33" s="88"/>
+      <c r="N33" s="88"/>
+      <c r="O33" s="88"/>
+      <c r="P33" s="88"/>
+      <c r="Q33" s="90"/>
+      <c r="R33" s="90"/>
+      <c r="S33" s="88"/>
+      <c r="T33" s="88"/>
+      <c r="U33" s="88"/>
+      <c r="V33" s="88"/>
+      <c r="W33" s="69"/>
+    </row>
+    <row r="34" spans="1:23" x14ac:dyDescent="0.4">
+      <c r="A34" s="88"/>
+      <c r="B34" s="88"/>
+      <c r="C34" s="89"/>
+      <c r="D34" s="88"/>
+      <c r="E34" s="88"/>
+      <c r="F34" s="88"/>
+      <c r="G34" s="88"/>
+      <c r="H34" s="88"/>
+      <c r="I34" s="88"/>
+      <c r="J34" s="88"/>
+      <c r="K34" s="88"/>
+      <c r="L34" s="88"/>
+      <c r="M34" s="88"/>
+      <c r="N34" s="88"/>
+      <c r="O34" s="88"/>
+      <c r="P34" s="88"/>
+      <c r="Q34" s="90"/>
+      <c r="R34" s="90"/>
+      <c r="S34" s="88"/>
+      <c r="T34" s="88"/>
+      <c r="U34" s="88"/>
+      <c r="V34" s="88"/>
+      <c r="W34" s="69"/>
+    </row>
+    <row r="35" spans="1:23" x14ac:dyDescent="0.4">
+      <c r="A35" s="88"/>
+      <c r="B35" s="90"/>
+      <c r="C35" s="89"/>
+      <c r="D35" s="88"/>
+      <c r="E35" s="88"/>
+      <c r="F35" s="88"/>
+      <c r="G35" s="88"/>
+      <c r="H35" s="88"/>
+      <c r="I35" s="88"/>
+      <c r="J35" s="88"/>
+      <c r="K35" s="88"/>
+      <c r="L35" s="88"/>
+      <c r="M35" s="88"/>
+      <c r="N35" s="88"/>
+      <c r="O35" s="88"/>
+      <c r="P35" s="88"/>
+      <c r="Q35" s="90"/>
+      <c r="R35" s="90"/>
+      <c r="S35" s="88"/>
+      <c r="T35" s="88"/>
+      <c r="U35" s="88"/>
+      <c r="V35" s="88"/>
+      <c r="W35" s="69"/>
+    </row>
+    <row r="36" spans="1:23" x14ac:dyDescent="0.4">
+      <c r="A36" s="88"/>
+      <c r="B36" s="90"/>
+      <c r="C36" s="89"/>
+      <c r="D36" s="88"/>
+      <c r="E36" s="88"/>
+      <c r="F36" s="88"/>
+      <c r="G36" s="88"/>
+      <c r="H36" s="88"/>
+      <c r="I36" s="88"/>
+      <c r="J36" s="88"/>
+      <c r="K36" s="88"/>
+      <c r="L36" s="88"/>
+      <c r="M36" s="88"/>
+      <c r="N36" s="88"/>
+      <c r="O36" s="88"/>
+      <c r="P36" s="88"/>
+      <c r="Q36" s="90"/>
+      <c r="R36" s="90"/>
+      <c r="S36" s="88"/>
+      <c r="T36" s="88"/>
+      <c r="U36" s="88"/>
+      <c r="V36" s="88"/>
+      <c r="W36" s="69"/>
+    </row>
+    <row r="37" spans="1:23" x14ac:dyDescent="0.4">
+      <c r="A37" s="88"/>
+      <c r="B37" s="90"/>
+      <c r="C37" s="89"/>
+      <c r="D37" s="88"/>
+      <c r="E37" s="88"/>
+      <c r="F37" s="88"/>
+      <c r="G37" s="88"/>
+      <c r="H37" s="88"/>
+      <c r="I37" s="88"/>
+      <c r="J37" s="88"/>
+      <c r="K37" s="88"/>
+      <c r="L37" s="88"/>
+      <c r="M37" s="88"/>
+      <c r="N37" s="88"/>
+      <c r="O37" s="88"/>
+      <c r="P37" s="88"/>
+      <c r="Q37" s="90"/>
+      <c r="R37" s="90"/>
+      <c r="S37" s="88"/>
+      <c r="T37" s="88"/>
+      <c r="U37" s="88"/>
+      <c r="V37" s="88"/>
+      <c r="W37" s="69"/>
+    </row>
+    <row r="38" spans="1:23" x14ac:dyDescent="0.4">
+      <c r="A38" s="86"/>
+      <c r="B38" s="86"/>
+      <c r="C38" s="86"/>
+      <c r="D38" s="86"/>
+      <c r="E38" s="86"/>
+      <c r="F38" s="86"/>
+      <c r="G38" s="86"/>
+      <c r="H38" s="86"/>
+      <c r="I38" s="86"/>
+      <c r="J38" s="86"/>
+      <c r="K38" s="86"/>
+      <c r="L38" s="86"/>
+      <c r="M38" s="86"/>
+      <c r="N38" s="86"/>
+      <c r="O38" s="86"/>
+      <c r="P38" s="86"/>
+      <c r="Q38" s="87"/>
+      <c r="R38" s="87"/>
+      <c r="S38" s="86"/>
+      <c r="T38" s="86"/>
+      <c r="U38" s="86"/>
+      <c r="V38" s="86"/>
     </row>
   </sheetData>
-  <mergeCells count="72">
-    <mergeCell ref="R17:R18"/>
-    <mergeCell ref="S19:V19"/>
-    <mergeCell ref="D19:P19"/>
-    <mergeCell ref="S1:V1"/>
-    <mergeCell ref="R3:R4"/>
-    <mergeCell ref="R5:R16"/>
-    <mergeCell ref="S9:V16"/>
-    <mergeCell ref="S32:V32"/>
-    <mergeCell ref="S22:V22"/>
-    <mergeCell ref="S23:V23"/>
-    <mergeCell ref="S24:V24"/>
-    <mergeCell ref="S25:V25"/>
-    <mergeCell ref="S26:V26"/>
-    <mergeCell ref="S20:V20"/>
-    <mergeCell ref="S21:V21"/>
-    <mergeCell ref="S17:V18"/>
-    <mergeCell ref="S33:V33"/>
-    <mergeCell ref="S34:V34"/>
-    <mergeCell ref="S35:V35"/>
-    <mergeCell ref="S36:V36"/>
-    <mergeCell ref="S27:V27"/>
-    <mergeCell ref="S28:V28"/>
-    <mergeCell ref="S29:V29"/>
-    <mergeCell ref="S30:V30"/>
-    <mergeCell ref="S31:V31"/>
-    <mergeCell ref="D35:P35"/>
-    <mergeCell ref="D36:P36"/>
-    <mergeCell ref="S2:V2"/>
-    <mergeCell ref="S3:V4"/>
-    <mergeCell ref="S5:V5"/>
-    <mergeCell ref="S6:V6"/>
-    <mergeCell ref="S7:V7"/>
-    <mergeCell ref="S8:V8"/>
-    <mergeCell ref="D30:P30"/>
-    <mergeCell ref="D31:P31"/>
-    <mergeCell ref="D32:P32"/>
-    <mergeCell ref="D33:P33"/>
-    <mergeCell ref="D34:P34"/>
-    <mergeCell ref="D25:P25"/>
-    <mergeCell ref="D26:P26"/>
-    <mergeCell ref="D27:P27"/>
-    <mergeCell ref="D28:P28"/>
-    <mergeCell ref="D29:P29"/>
-    <mergeCell ref="D20:P20"/>
+  <mergeCells count="45">
+    <mergeCell ref="D2:P2"/>
+    <mergeCell ref="A1:Q1"/>
+    <mergeCell ref="D10:P10"/>
+    <mergeCell ref="D3:P4"/>
+    <mergeCell ref="Q3:Q4"/>
+    <mergeCell ref="D6:P6"/>
+    <mergeCell ref="D7:P7"/>
+    <mergeCell ref="D8:P8"/>
+    <mergeCell ref="D9:P9"/>
+    <mergeCell ref="C5:V5"/>
+    <mergeCell ref="S22:V25"/>
+    <mergeCell ref="B22:B25"/>
+    <mergeCell ref="A5:A25"/>
+    <mergeCell ref="B6:B21"/>
+    <mergeCell ref="A3:A4"/>
+    <mergeCell ref="B3:B4"/>
     <mergeCell ref="D21:P21"/>
     <mergeCell ref="D22:P22"/>
     <mergeCell ref="D23:P23"/>
     <mergeCell ref="D24:P24"/>
-    <mergeCell ref="D15:P15"/>
+    <mergeCell ref="D25:P25"/>
+    <mergeCell ref="S2:V2"/>
+    <mergeCell ref="S3:V4"/>
+    <mergeCell ref="S6:V6"/>
+    <mergeCell ref="S7:V7"/>
+    <mergeCell ref="S8:V8"/>
+    <mergeCell ref="S9:V9"/>
+    <mergeCell ref="S21:V21"/>
+    <mergeCell ref="S18:V19"/>
+    <mergeCell ref="R18:R19"/>
+    <mergeCell ref="S20:V20"/>
+    <mergeCell ref="D20:P20"/>
+    <mergeCell ref="S1:V1"/>
+    <mergeCell ref="R3:R4"/>
+    <mergeCell ref="R6:R17"/>
+    <mergeCell ref="S10:V17"/>
     <mergeCell ref="D16:P16"/>
     <mergeCell ref="D17:P17"/>
     <mergeCell ref="D18:P18"/>
-    <mergeCell ref="D10:P10"/>
+    <mergeCell ref="D19:P19"/>
     <mergeCell ref="D11:P11"/>
     <mergeCell ref="D12:P12"/>
     <mergeCell ref="D13:P13"/>
     <mergeCell ref="D14:P14"/>
-    <mergeCell ref="A21:A36"/>
-    <mergeCell ref="A5:A20"/>
-    <mergeCell ref="B5:B20"/>
-    <mergeCell ref="A3:A4"/>
-    <mergeCell ref="B3:B4"/>
-    <mergeCell ref="B21:B33"/>
-    <mergeCell ref="D2:P2"/>
-    <mergeCell ref="A1:Q1"/>
-    <mergeCell ref="D9:P9"/>
-    <mergeCell ref="D3:P4"/>
-    <mergeCell ref="Q3:Q4"/>
-    <mergeCell ref="D5:P5"/>
-    <mergeCell ref="D6:P6"/>
-    <mergeCell ref="D7:P7"/>
-    <mergeCell ref="D8:P8"/>
+    <mergeCell ref="D15:P15"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>